<commit_message>
Sheet Name, ListObject Name에 #으로 시작할 경우 제외
</commit_message>
<xml_diff>
--- a/TestExcel/GameData.xlsx
+++ b/TestExcel/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
   <si>
     <t>Enum</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,15 +179,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>#int32_cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#int32_cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Param_1 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Param_1 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>#으로 시작하는 컬럼은 제외</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#Param_1 설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Param_1 설명</t>
+    <t>#으로 시작하는 컬럼은 제외</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -679,7 +691,7 @@
   <dimension ref="B2:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -722,7 +734,7 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K2" t="s">
         <v>30</v>
@@ -763,7 +775,7 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
         <v>11</v>
@@ -804,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -883,7 +895,7 @@
         <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
         <v>30</v>
@@ -924,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
         <v>11</v>
@@ -963,6 +975,9 @@
       </c>
       <c r="I11">
         <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -992,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1052,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
         <v>30</v>

</xml_diff>